<commit_message>
no idea, it was waiting for commit on my laptop
</commit_message>
<xml_diff>
--- a/functionaldiv2012_newtraits.xlsx
+++ b/functionaldiv2012_newtraits.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emily\Documents\Dissertation\DissertationScripts\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="360" yWindow="135" windowWidth="16275" windowHeight="10545"/>
   </bookViews>
   <sheets>
     <sheet name="functionaldiv2012_newtraits" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -732,6 +737,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -852,21 +860,22 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="70449664"/>
-        <c:axId val="75365696"/>
+        <c:gapWidth val="57"/>
+        <c:axId val="297856512"/>
+        <c:axId val="297856904"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="70449664"/>
+        <c:axId val="297856512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75365696"/>
+        <c:crossAx val="297856904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -874,9 +883,11 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="75365696"/>
+        <c:axId val="297856904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -884,7 +895,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70449664"/>
+        <c:crossAx val="297856512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -913,13 +924,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>514349</xdr:colOff>
+      <xdr:colOff>514350</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>485774</xdr:colOff>
+      <xdr:colOff>123826</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
@@ -986,7 +997,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1021,7 +1032,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1232,8 +1243,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>